<commit_message>
Finialized Bill of Materials with sample components/links
</commit_message>
<xml_diff>
--- a/BadgersHollowSchematic/Badgers Hollow BOE.xlsx
+++ b/BadgersHollowSchematic/Badgers Hollow BOE.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spencer\Desktop\projects\BadgersHollow\BadgersHollowSchematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C829C3D2-6B38-4A9B-B574-8667875CD42D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B7B6C3-14CA-4804-B47B-80B45A788D91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9BD8A107-303F-4A99-A03A-7F536F09A5B1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9BD8A107-303F-4A99-A03A-7F536F09A5B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Badgers Hollow BOE" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Badgers Hollow BOE'!$A$1:$M$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -104,21 +107,12 @@
     <t>22pF 1206 Cap for the oscillator</t>
   </si>
   <si>
-    <t>https://www.mouser.com/datasheet/2/396/taiyo_yuden_07182019_MLCC_AECQ200_Grade_1_X7R_data-1622917.pdf</t>
-  </si>
-  <si>
     <t>1uF cap for ucap</t>
   </si>
   <si>
     <t>C3</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Taiyo-Yuden/EMF316B7105KLHT?qs=%252B6g0mu59x7JIndjmt7B12g%3D%3D</t>
-  </si>
-  <si>
-    <t>EMF316B7105KLHT</t>
-  </si>
-  <si>
     <t>http://ww1.microchip.com/downloads/en/DeviceDoc/Atmel-7766-8-bit-AVR-ATmega16U4-32U4_Datasheet.pdf</t>
   </si>
   <si>
@@ -212,12 +206,6 @@
     <t>https://www.mouser.com/datasheet/2/396/mlcc02_e-1307760.pdf</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Taiyo-Yuden/JMK107ABJ106KAHT?qs=sGAEpiMZZMvsSlwiRhF8qtsGU%2FCnaNeQsMTp5MAa%252B9ZwWVhFkL79AQ%3D%3D</t>
-  </si>
-  <si>
-    <t>JMK107ABJ106KAHT</t>
-  </si>
-  <si>
     <t>SW27</t>
   </si>
   <si>
@@ -360,6 +348,21 @@
   </si>
   <si>
     <t>CC0805KRX7R6BB104</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Taiyo-Yuden/JMK107ABJ106KA-T?qs=sGAEpiMZZMvsSlwiRhF8qvXH2%252BT6Wjq15yN1ctyCMjv%2FxorzUyDEbQ%3D%3D</t>
+  </si>
+  <si>
+    <t>JMK107ABJ106KA-T</t>
+  </si>
+  <si>
+    <t>C1206C105K3RACTU</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/C1206C105K3RACTU?qs=sGAEpiMZZMvsSlwiRhF8qoWac7aB9v08aZfRC70hdIk%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/212/KEM_C1002_X7R_SMD-1102033.pdf</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -441,6 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -758,8 +762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EED7D3-EBE2-4140-9EBC-E72AB61D2917}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,11 +813,11 @@
         <v>16</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M1">
         <f>SUM(E:E)</f>
-        <v>30.938000000000002</v>
+        <v>30.738</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -856,7 +861,7 @@
         <v>0.46</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E22" si="0">D3*C3</f>
+        <f t="shared" ref="E3:E20" si="0">D3*C3</f>
         <v>0.46</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -875,7 +880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -896,7 +901,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2">
         <v>1206</v>
@@ -908,37 +913,37 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
+      <c r="B5" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>0.31</v>
+        <v>0.26</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0.31</v>
+        <v>0.26</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="2">
         <v>1206</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>26</v>
+        <v>108</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -946,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -959,19 +964,19 @@
         <v>1.31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -979,7 +984,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -992,19 +997,19 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1012,7 +1017,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1025,19 +1030,19 @@
         <v>0.15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8" s="2">
         <v>1206</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1045,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1058,19 +1063,19 @@
         <v>0.4</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H9" s="2">
         <v>1206</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1078,7 +1083,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -1091,52 +1096,52 @@
         <v>0.36</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H10" s="2">
         <v>805</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>60</v>
+      <c r="B11" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H11" s="2">
         <v>603</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1144,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1157,19 +1162,19 @@
         <v>4.5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1177,7 +1182,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -1190,19 +1195,19 @@
         <v>0.35</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1210,7 +1215,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
@@ -1223,19 +1228,19 @@
         <v>1.26</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H14" s="2">
         <v>1206</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1243,7 +1248,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -1256,19 +1261,19 @@
         <v>0.11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H15" s="2">
         <v>1206</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1276,7 +1281,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2">
         <v>2</v>
@@ -1289,19 +1294,19 @@
         <v>0.4</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H16" s="2">
         <v>805</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1309,7 +1314,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
@@ -1322,19 +1327,19 @@
         <v>0.76</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1342,7 +1347,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C18" s="2">
         <v>24</v>
@@ -1355,19 +1360,19 @@
         <v>4.08</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1375,7 +1380,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C19" s="2">
         <v>2</v>
@@ -1388,16 +1393,16 @@
         <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1405,7 +1410,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C20" s="2">
         <v>22</v>
@@ -1418,27 +1423,30 @@
         <v>3.08</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H20" s="2">
         <v>805</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{3F375582-380B-4EA6-A58A-E6B9358F7F8B}"/>
     <hyperlink ref="J4" r:id="rId2" xr:uid="{C4D80F7A-50FF-407C-A7AF-A4F1733F1F5C}"/>
+    <hyperlink ref="B11" r:id="rId3" display="https://www.mouser.com/ProductDetail/Taiyo-Yuden/JMK107ABJ106KA-T?qs=sGAEpiMZZMvsSlwiRhF8qvXH2%252BT6Wjq15yN1ctyCMjv%2FxorzUyDEbQ%3D%3D" xr:uid="{FC30D687-BC3B-44F3-AAAB-3EF0FAEC5B08}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.mouser.com/ProductDetail/KEMET/C1206C105K3RACTU?qs=sGAEpiMZZMvsSlwiRhF8qoWac7aB9v08aZfRC70hdIk%3D" xr:uid="{C3C31E51-12B9-4E99-BAA3-E3FC886367AA}"/>
+    <hyperlink ref="J5" r:id="rId5" xr:uid="{AF7BBF72-9214-4B1A-A1E1-E3646D2C71F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>